<commit_message>
2021.08.14  细节修订 Preview 2 版本
</commit_message>
<xml_diff>
--- a/概要.xlsx
+++ b/概要.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QTProject\qETRC\qETRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8ACA5A-8F1C-4A82-8503-0BCDF378FD5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7B6135-69F2-4522-91A9-01816C8487DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{2D193B45-5A4E-46CA-B003-4706E03AE908}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2D193B45-5A4E-46CA-B003-4706E03AE908}"/>
   </bookViews>
   <sheets>
     <sheet name="操作命令表" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="192">
   <si>
     <t>qETRC操作命令总表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -736,10 +736,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>更新标尺数据，或者是否上下行分设</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>完成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -753,6 +749,54 @@
   </si>
   <si>
     <t>完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除标尺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RemoveRuler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除指定标尺，如果是排图标尺，同时把该线路排图标尺设为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更改标尺名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChangeRulerName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改标尺的名称（但数据不变）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新标尺数据，或者是否上下行分设（但名称不变）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新建空白标尺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddNewRuler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加空白标尺，同时打开编辑面板</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1145,11 +1189,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5840A104-B5EE-45CC-B3E0-544B00077931}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1656,17 +1700,70 @@
         <v>44399</v>
       </c>
       <c r="G23" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
+      <c r="B24" t="s">
+        <v>185</v>
+      </c>
+      <c r="C24" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" t="s">
+        <v>182</v>
+      </c>
+      <c r="E24" t="s">
+        <v>183</v>
+      </c>
+      <c r="G24" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>180</v>
+      </c>
+      <c r="C25" t="s">
+        <v>181</v>
+      </c>
+      <c r="D25" t="s">
+        <v>182</v>
+      </c>
+      <c r="E25" t="s">
+        <v>183</v>
+      </c>
+      <c r="G25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" t="s">
+        <v>190</v>
+      </c>
+      <c r="D26" t="s">
+        <v>182</v>
+      </c>
+      <c r="E26" t="s">
+        <v>183</v>
+      </c>
+      <c r="F26" s="1">
+        <v>44422</v>
+      </c>
+      <c r="G26" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -1920,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB65AA12-ED68-4484-9C2E-07111EA4714A}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2184,7 +2281,7 @@
         <v>171</v>
       </c>
       <c r="C30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2200,20 +2297,20 @@
         <v>173</v>
       </c>
       <c r="C32" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>178</v>
+      </c>
+      <c r="C34" t="s">
         <v>179</v>
-      </c>
-      <c r="C34" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023.01.21  basically finished for: editting support for PredefTrainFilter
</commit_message>
<xml_diff>
--- a/概要.xlsx
+++ b/概要.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QTProject\qETRC\qETRC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codes\QtProjects\qETRC\qETRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32EF36D-B541-4483-952B-97378F8DE66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40EAC4E-2E96-4C0C-BC50-D25ED5C78505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2D193B45-5A4E-46CA-B003-4706E03AE908}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{2D193B45-5A4E-46CA-B003-4706E03AE908}"/>
   </bookViews>
   <sheets>
     <sheet name="操作命令表" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="309">
   <si>
     <t>qETRC操作命令总表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1241,6 +1241,30 @@
   </si>
   <si>
     <t>和ChangePageConfig的实质行为一致，但支持操作合并</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新建预置列车筛选器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddTrainFilter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除预置列车筛选器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RemoveTrainFilter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新列车筛选器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UpdateTrainFilter</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1628,7 +1652,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1636,27 +1660,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5840A104-B5EE-45CC-B3E0-544B00077931}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
+      <selection pane="bottomLeft" activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="3" max="3" width="24.21875" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.4140625" customWidth="1"/>
+    <col min="3" max="3" width="24.25" customWidth="1"/>
+    <col min="6" max="6" width="16.4140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1679,7 +1703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1702,7 +1726,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1725,7 +1749,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1748,7 +1772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1771,7 +1795,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1794,7 +1818,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1814,7 +1838,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1834,7 +1858,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1857,7 +1881,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1880,7 +1904,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1903,7 +1927,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1923,7 +1947,7 @@
         <v>44386</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1946,7 +1970,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1969,7 +1993,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1992,7 +2016,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2015,7 +2039,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2038,7 +2062,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2061,7 +2085,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2084,7 +2108,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2107,7 +2131,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2130,7 +2154,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2153,7 +2177,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2173,7 +2197,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2193,7 +2217,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2216,7 +2240,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2239,7 +2263,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2262,7 +2286,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2285,7 +2309,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2308,7 +2332,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2331,7 +2355,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2354,7 +2378,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2377,7 +2401,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2400,7 +2424,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2423,7 +2447,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2446,7 +2470,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2469,7 +2493,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2492,7 +2516,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2506,7 +2530,7 @@
         <v>44442</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2529,7 +2553,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2552,7 +2576,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2575,7 +2599,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2595,7 +2619,7 @@
         <v>44454</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2615,7 +2639,7 @@
         <v>44454</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2635,7 +2659,7 @@
         <v>44454</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2655,7 +2679,7 @@
         <v>44454</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2678,7 +2702,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2698,7 +2722,7 @@
         <v>44455</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2718,7 +2742,7 @@
         <v>44455</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2738,7 +2762,7 @@
         <v>44455</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2758,7 +2782,7 @@
         <v>44455</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2778,7 +2802,7 @@
         <v>44455</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2801,7 +2825,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2824,7 +2848,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2844,7 +2868,7 @@
         <v>44478</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2867,7 +2891,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2890,7 +2914,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2913,9 +2937,64 @@
         <v>302</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>303</v>
+      </c>
+      <c r="C59" t="s">
+        <v>304</v>
+      </c>
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" t="s">
+        <v>56</v>
+      </c>
+      <c r="F59" s="1">
+        <v>44947</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>305</v>
+      </c>
+      <c r="C60" t="s">
+        <v>306</v>
+      </c>
+      <c r="D60" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" t="s">
+        <v>56</v>
+      </c>
+      <c r="F60" s="1">
+        <v>44947</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>307</v>
+      </c>
+      <c r="C61" t="s">
+        <v>308</v>
+      </c>
+      <c r="D61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" t="s">
+        <v>56</v>
+      </c>
+      <c r="F61" s="1">
+        <v>44947</v>
       </c>
     </row>
   </sheetData>
@@ -2937,17 +3016,17 @@
       <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>47</v>
       </c>
@@ -2961,22 +3040,22 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2984,12 +3063,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2997,17 +3076,17 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -3015,27 +3094,27 @@
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -3043,7 +3122,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -3051,12 +3130,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -3064,7 +3143,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -3072,7 +3151,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -3080,12 +3159,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -3093,22 +3172,22 @@
         <v>244</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -3116,7 +3195,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -3124,52 +3203,52 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>0</v>
       </c>
@@ -3188,22 +3267,22 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -3214,7 +3293,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>76</v>
       </c>
@@ -3222,7 +3301,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>77</v>
       </c>
@@ -3230,7 +3309,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>78</v>
       </c>
@@ -3241,7 +3320,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -3252,7 +3331,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>85</v>
       </c>
@@ -3260,7 +3339,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -3268,7 +3347,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>104</v>
       </c>
@@ -3276,7 +3355,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>86</v>
       </c>
@@ -3284,7 +3363,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>89</v>
       </c>
@@ -3292,7 +3371,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>90</v>
       </c>
@@ -3300,7 +3379,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -3311,7 +3390,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>91</v>
       </c>
@@ -3319,7 +3398,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>92</v>
       </c>
@@ -3327,7 +3406,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -3335,7 +3414,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>119</v>
       </c>
@@ -3343,7 +3422,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>121</v>
       </c>
@@ -3351,7 +3430,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -3362,7 +3441,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>102</v>
       </c>
@@ -3370,7 +3449,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>103</v>
       </c>
@@ -3378,7 +3457,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -3389,7 +3468,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -3400,7 +3479,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>99</v>
       </c>
@@ -3408,7 +3487,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>152</v>
       </c>
@@ -3416,7 +3495,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>153</v>
       </c>
@@ -3424,7 +3503,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>96</v>
       </c>
@@ -3432,7 +3511,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>166</v>
       </c>
@@ -3443,7 +3522,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>168</v>
       </c>
@@ -3451,7 +3530,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>169</v>
       </c>
@@ -3459,7 +3538,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>170</v>
       </c>
@@ -3467,12 +3546,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>175</v>
       </c>

</xml_diff>

<commit_message>
2023.02.04  add entrance for TimetableInterpSimple in TrainContext; release V1.3.2 R36
</commit_message>
<xml_diff>
--- a/概要.xlsx
+++ b/概要.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codes\QtProjects\qETRC\qETRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40EAC4E-2E96-4C0C-BC50-D25ED5C78505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9772B97B-B532-42F8-A6F9-DDF9AF1C8A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{2D193B45-5A4E-46CA-B003-4706E03AE908}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="312">
   <si>
     <t>qETRC操作命令总表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1265,6 +1265,18 @@
   </si>
   <si>
     <t>UpdateTrainFilter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时刻表快速插值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TimetableInterpolationSimple</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>和ChangeTimetable实质上一致。快速推定列车在本线的跨越站时刻。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1652,7 +1664,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1660,11 +1672,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5840A104-B5EE-45CC-B3E0-544B00077931}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G61" sqref="G61"/>
+      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2995,6 +3007,29 @@
       </c>
       <c r="F61" s="1">
         <v>44947</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>309</v>
+      </c>
+      <c r="C62" t="s">
+        <v>310</v>
+      </c>
+      <c r="D62" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" t="s">
+        <v>56</v>
+      </c>
+      <c r="F62" s="1">
+        <v>44960</v>
+      </c>
+      <c r="G62" t="s">
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023.06.02  basically tests passed for Dragging
</commit_message>
<xml_diff>
--- a/概要.xlsx
+++ b/概要.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codes\QtProjects\qETRC\qETRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9772B97B-B532-42F8-A6F9-DDF9AF1C8A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEB6D98-1DF1-44AE-8E60-B52D1142C257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{2D193B45-5A4E-46CA-B003-4706E03AE908}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="316">
   <si>
     <t>qETRC操作命令总表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -252,18 +252,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>操作合并</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>否</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>更新基线数据</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1236,10 +1228,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>和ChangePageConfig的实质行为一致，但支持操作合并</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1277,6 +1265,34 @@
   </si>
   <si>
     <t>和ChangeTimetable实质上一致。快速推定列车在本线的跨越站时刻。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拖动时刻</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DragTrainStationTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>和AdjustTrainStationTime类似，拖动调整单个车站时刻</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>列车时刻微调</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AdjustTrainStationTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>速览时刻中微调时刻（本行补档）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>操作合并ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1672,11 +1688,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5840A104-B5EE-45CC-B3E0-544B00077931}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1706,7 +1722,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>315</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>6</v>
@@ -1729,7 +1745,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" s="1">
         <v>44379</v>
@@ -1752,7 +1768,7 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F4" s="1">
         <v>44379</v>
@@ -1775,7 +1791,7 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" s="1">
         <v>44380</v>
@@ -1797,8 +1813,8 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>57</v>
+      <c r="E6" s="2">
+        <v>100</v>
       </c>
       <c r="F6" s="1">
         <v>44380</v>
@@ -1812,22 +1828,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
         <v>58</v>
       </c>
-      <c r="C7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" t="s">
-        <v>60</v>
-      </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" s="1">
         <v>44381</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1835,19 +1851,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="F8" s="1">
         <v>44381</v>
       </c>
       <c r="G8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1855,19 +1871,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F9" s="1">
         <v>44381</v>
       </c>
       <c r="G9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1875,22 +1891,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
         <v>66</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>67</v>
-      </c>
-      <c r="D10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" t="s">
-        <v>69</v>
       </c>
       <c r="F10" s="1">
         <v>44382</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1898,22 +1914,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F11" s="1">
         <v>44382</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1921,22 +1937,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" t="s">
         <v>106</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>107</v>
-      </c>
-      <c r="D12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" t="s">
-        <v>109</v>
       </c>
       <c r="F12" s="1">
         <v>44385</v>
       </c>
       <c r="G12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1944,16 +1960,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F13" s="1">
         <v>44386</v>
@@ -1964,22 +1980,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" t="s">
         <v>113</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>114</v>
-      </c>
-      <c r="D14" t="s">
-        <v>115</v>
-      </c>
-      <c r="E14" t="s">
-        <v>116</v>
       </c>
       <c r="F14" s="1">
         <v>44386</v>
       </c>
       <c r="G14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1987,22 +2003,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" t="s">
         <v>121</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
         <v>122</v>
-      </c>
-      <c r="D15" t="s">
-        <v>123</v>
-      </c>
-      <c r="E15" t="s">
-        <v>124</v>
       </c>
       <c r="F15" s="1">
         <v>44387</v>
       </c>
       <c r="G15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2010,22 +2026,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F16" s="1">
         <v>44387</v>
       </c>
       <c r="G16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -2033,22 +2049,22 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" t="s">
         <v>131</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
         <v>132</v>
-      </c>
-      <c r="D17" t="s">
-        <v>133</v>
-      </c>
-      <c r="E17" t="s">
-        <v>134</v>
       </c>
       <c r="F17" s="1">
         <v>44388</v>
       </c>
       <c r="G17" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -2056,22 +2072,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" t="s">
         <v>137</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>138</v>
-      </c>
-      <c r="D18" t="s">
-        <v>139</v>
-      </c>
-      <c r="E18" t="s">
-        <v>140</v>
       </c>
       <c r="F18" s="1">
         <v>44388</v>
       </c>
       <c r="G18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -2079,22 +2095,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F19" s="4">
         <v>44484</v>
       </c>
       <c r="G19" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -2102,22 +2118,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" t="s">
+        <v>143</v>
+      </c>
+      <c r="D20" t="s">
         <v>144</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>145</v>
-      </c>
-      <c r="D20" t="s">
-        <v>146</v>
-      </c>
-      <c r="E20" t="s">
-        <v>147</v>
       </c>
       <c r="F20" s="1">
         <v>44390</v>
       </c>
       <c r="G20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -2125,22 +2141,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" t="s">
         <v>154</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>155</v>
-      </c>
-      <c r="D21" t="s">
-        <v>156</v>
-      </c>
-      <c r="E21" t="s">
-        <v>157</v>
       </c>
       <c r="F21" s="1">
         <v>44391</v>
       </c>
       <c r="G21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -2148,22 +2164,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" t="s">
         <v>160</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
         <v>161</v>
-      </c>
-      <c r="D22" t="s">
-        <v>162</v>
-      </c>
-      <c r="E22" t="s">
-        <v>163</v>
       </c>
       <c r="F22" s="1">
         <v>44392</v>
       </c>
       <c r="G22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -2171,22 +2187,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F23" s="1">
         <v>44399</v>
       </c>
       <c r="G23" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -2194,19 +2210,19 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>180</v>
+      </c>
+      <c r="C24" t="s">
+        <v>181</v>
+      </c>
+      <c r="D24" t="s">
+        <v>177</v>
+      </c>
+      <c r="E24" t="s">
+        <v>178</v>
+      </c>
+      <c r="G24" t="s">
         <v>182</v>
-      </c>
-      <c r="C24" t="s">
-        <v>183</v>
-      </c>
-      <c r="D24" t="s">
-        <v>179</v>
-      </c>
-      <c r="E24" t="s">
-        <v>180</v>
-      </c>
-      <c r="G24" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -2214,19 +2230,19 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>175</v>
+      </c>
+      <c r="C25" t="s">
+        <v>176</v>
+      </c>
+      <c r="D25" t="s">
         <v>177</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>178</v>
       </c>
-      <c r="D25" t="s">
+      <c r="G25" t="s">
         <v>179</v>
-      </c>
-      <c r="E25" t="s">
-        <v>180</v>
-      </c>
-      <c r="G25" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -2234,22 +2250,22 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C26" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D26" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F26" s="1">
         <v>44422</v>
       </c>
       <c r="G26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -2257,22 +2273,22 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
+        <v>187</v>
+      </c>
+      <c r="C27" t="s">
+        <v>188</v>
+      </c>
+      <c r="D27" t="s">
         <v>189</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>190</v>
-      </c>
-      <c r="D27" t="s">
-        <v>191</v>
-      </c>
-      <c r="E27" t="s">
-        <v>192</v>
       </c>
       <c r="F27" s="1">
         <v>44423</v>
       </c>
       <c r="G27" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -2280,22 +2296,22 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>192</v>
+      </c>
+      <c r="C28" t="s">
+        <v>193</v>
+      </c>
+      <c r="D28" t="s">
         <v>194</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>195</v>
-      </c>
-      <c r="D28" t="s">
-        <v>196</v>
-      </c>
-      <c r="E28" t="s">
-        <v>197</v>
       </c>
       <c r="F28" s="1">
         <v>44427</v>
       </c>
       <c r="G28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -2303,22 +2319,22 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
+        <v>197</v>
+      </c>
+      <c r="C29" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" t="s">
         <v>199</v>
       </c>
-      <c r="C29" t="s">
+      <c r="E29" t="s">
         <v>200</v>
-      </c>
-      <c r="D29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E29" t="s">
-        <v>202</v>
       </c>
       <c r="F29" s="1">
         <v>44428</v>
       </c>
       <c r="G29" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -2326,22 +2342,22 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C30" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D30" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F30" s="1">
         <v>44430</v>
       </c>
       <c r="G30" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -2349,22 +2365,22 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
+        <v>205</v>
+      </c>
+      <c r="C31" t="s">
+        <v>206</v>
+      </c>
+      <c r="D31" t="s">
         <v>207</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>208</v>
-      </c>
-      <c r="D31" t="s">
-        <v>209</v>
-      </c>
-      <c r="E31" t="s">
-        <v>210</v>
       </c>
       <c r="F31" s="1">
         <v>44432</v>
       </c>
       <c r="G31" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -2372,22 +2388,22 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
+        <v>210</v>
+      </c>
+      <c r="C32" t="s">
+        <v>211</v>
+      </c>
+      <c r="D32" t="s">
         <v>212</v>
       </c>
-      <c r="C32" t="s">
+      <c r="E32" t="s">
         <v>213</v>
-      </c>
-      <c r="D32" t="s">
-        <v>214</v>
-      </c>
-      <c r="E32" t="s">
-        <v>215</v>
       </c>
       <c r="F32" s="1">
         <v>44433</v>
       </c>
       <c r="G32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2395,22 +2411,22 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C33" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D33" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E33" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F33" s="1">
         <v>44434</v>
       </c>
       <c r="G33" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2418,22 +2434,22 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C34" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D34" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E34" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F34" s="1">
         <v>44435</v>
       </c>
       <c r="G34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2441,22 +2457,22 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C35" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D35" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E35" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F35" s="1">
         <v>44435</v>
       </c>
       <c r="G35" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2464,22 +2480,22 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
+        <v>224</v>
+      </c>
+      <c r="C36" t="s">
+        <v>225</v>
+      </c>
+      <c r="D36" t="s">
         <v>226</v>
       </c>
-      <c r="C36" t="s">
+      <c r="E36" t="s">
         <v>227</v>
-      </c>
-      <c r="D36" t="s">
-        <v>228</v>
-      </c>
-      <c r="E36" t="s">
-        <v>229</v>
       </c>
       <c r="F36" s="1">
         <v>44439</v>
       </c>
       <c r="G36" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2487,22 +2503,22 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C37" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D37" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E37" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F37" s="1">
         <v>44439</v>
       </c>
       <c r="G37" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2510,22 +2526,22 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
+        <v>232</v>
+      </c>
+      <c r="C38" t="s">
+        <v>233</v>
+      </c>
+      <c r="D38" t="s">
         <v>234</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E38" t="s">
         <v>235</v>
-      </c>
-      <c r="D38" t="s">
-        <v>236</v>
-      </c>
-      <c r="E38" t="s">
-        <v>237</v>
       </c>
       <c r="F38" s="1">
         <v>44441</v>
       </c>
       <c r="G38" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2533,10 +2549,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F39" s="1">
         <v>44442</v>
@@ -2547,22 +2563,22 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
+        <v>244</v>
+      </c>
+      <c r="C40" t="s">
+        <v>245</v>
+      </c>
+      <c r="D40" t="s">
         <v>246</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" t="s">
         <v>247</v>
-      </c>
-      <c r="D40" t="s">
-        <v>248</v>
-      </c>
-      <c r="E40" t="s">
-        <v>249</v>
       </c>
       <c r="F40" s="1">
         <v>44444</v>
       </c>
       <c r="G40" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -2570,22 +2586,22 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
+        <v>249</v>
+      </c>
+      <c r="C41" t="s">
+        <v>250</v>
+      </c>
+      <c r="D41" t="s">
         <v>251</v>
       </c>
-      <c r="C41" t="s">
+      <c r="E41" t="s">
         <v>252</v>
-      </c>
-      <c r="D41" t="s">
-        <v>253</v>
-      </c>
-      <c r="E41" t="s">
-        <v>254</v>
       </c>
       <c r="F41" s="1">
         <v>44450</v>
       </c>
       <c r="G41" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -2593,22 +2609,22 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
+        <v>254</v>
+      </c>
+      <c r="C42" t="s">
+        <v>255</v>
+      </c>
+      <c r="D42" t="s">
         <v>256</v>
       </c>
-      <c r="C42" t="s">
+      <c r="E42" t="s">
         <v>257</v>
-      </c>
-      <c r="D42" t="s">
-        <v>258</v>
-      </c>
-      <c r="E42" t="s">
-        <v>259</v>
       </c>
       <c r="F42" s="1">
         <v>44453</v>
       </c>
       <c r="G42" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2616,16 +2632,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C43" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D43" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E43" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F43" s="1">
         <v>44454</v>
@@ -2636,16 +2652,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C44" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D44" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E44" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F44" s="1">
         <v>44454</v>
@@ -2656,16 +2672,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C45" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D45" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E45" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F45" s="1">
         <v>44454</v>
@@ -2676,16 +2692,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C46" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D46" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E46" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F46" s="1">
         <v>44454</v>
@@ -2696,22 +2712,22 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C47" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D47" t="s">
         <v>9</v>
       </c>
       <c r="E47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F47" s="1">
         <v>44455</v>
       </c>
       <c r="G47" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -2719,16 +2735,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C48" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D48" t="s">
         <v>9</v>
       </c>
       <c r="E48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F48" s="1">
         <v>44455</v>
@@ -2739,16 +2755,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C49" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D49" t="s">
         <v>9</v>
       </c>
       <c r="E49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F49" s="1">
         <v>44455</v>
@@ -2759,16 +2775,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C50" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D50" t="s">
         <v>9</v>
       </c>
       <c r="E50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F50" s="1">
         <v>44455</v>
@@ -2779,16 +2795,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C51" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D51" t="s">
         <v>9</v>
       </c>
       <c r="E51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F51" s="1">
         <v>44455</v>
@@ -2799,16 +2815,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C52" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D52" t="s">
         <v>9</v>
       </c>
       <c r="E52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F52" s="1">
         <v>44455</v>
@@ -2819,22 +2835,22 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C53" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D53" t="s">
         <v>9</v>
       </c>
       <c r="E53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F53" s="1">
         <v>44459</v>
       </c>
       <c r="G53" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -2842,22 +2858,22 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C54" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D54" t="s">
         <v>9</v>
       </c>
       <c r="E54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F54" s="1">
         <v>44477</v>
       </c>
       <c r="G54" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -2865,16 +2881,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C55" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D55" t="s">
         <v>9</v>
       </c>
       <c r="E55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F55" s="1">
         <v>44478</v>
@@ -2885,22 +2901,22 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C56" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D56" t="s">
         <v>9</v>
       </c>
       <c r="E56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F56" s="1">
         <v>44484</v>
       </c>
       <c r="G56" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -2908,22 +2924,22 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C57" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D57" t="s">
         <v>9</v>
       </c>
       <c r="E57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F57" s="1">
         <v>44598</v>
       </c>
       <c r="G57" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -2931,22 +2947,22 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C58" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D58" t="s">
         <v>9</v>
       </c>
-      <c r="E58" s="2" t="s">
-        <v>301</v>
+      <c r="E58" s="2">
+        <v>102</v>
       </c>
       <c r="F58" s="1">
         <v>44703</v>
       </c>
       <c r="G58" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -2954,16 +2970,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C59" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D59" t="s">
         <v>9</v>
       </c>
       <c r="E59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F59" s="1">
         <v>44947</v>
@@ -2974,16 +2990,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C60" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D60" t="s">
         <v>9</v>
       </c>
       <c r="E60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F60" s="1">
         <v>44947</v>
@@ -2994,16 +3010,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C61" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D61" t="s">
         <v>9</v>
       </c>
       <c r="E61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F61" s="1">
         <v>44947</v>
@@ -3014,21 +3030,64 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C62" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D62" t="s">
         <v>9</v>
       </c>
       <c r="E62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F62" s="1">
         <v>44960</v>
       </c>
       <c r="G62" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>312</v>
+      </c>
+      <c r="C63" t="s">
+        <v>313</v>
+      </c>
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="2">
+        <v>101</v>
+      </c>
+      <c r="G63" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>309</v>
+      </c>
+      <c r="C64" t="s">
+        <v>310</v>
+      </c>
+      <c r="D64" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="2">
+        <v>103</v>
+      </c>
+      <c r="F64" s="1">
+        <v>45079</v>
+      </c>
+      <c r="G64" t="s">
         <v>311</v>
       </c>
     </row>
@@ -3095,7 +3154,7 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -3108,7 +3167,7 @@
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -3126,7 +3185,7 @@
         <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -3175,7 +3234,7 @@
         <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -3183,7 +3242,7 @@
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -3204,7 +3263,7 @@
         <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -3309,69 +3368,69 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -3379,66 +3438,66 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -3446,152 +3505,152 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C27" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C29" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C30" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C31" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C32" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C34" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023.08.12  basic framework for addition/deletion of TrainPaths
</commit_message>
<xml_diff>
--- a/概要.xlsx
+++ b/概要.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codes\QtProjects\qETRC\qETRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEB6D98-1DF1-44AE-8E60-B52D1142C257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFAD795-A8FC-4445-8539-EA39BE365630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{2D193B45-5A4E-46CA-B003-4706E03AE908}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="321">
   <si>
     <t>qETRC操作命令总表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1293,6 +1293,26 @@
   </si>
   <si>
     <t>操作合并ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加列车径路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddTrainPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除列车径路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RemoveTrainPath</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1688,11 +1708,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5840A104-B5EE-45CC-B3E0-544B00077931}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3089,6 +3109,46 @@
       </c>
       <c r="G64" t="s">
         <v>311</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>316</v>
+      </c>
+      <c r="C65" t="s">
+        <v>317</v>
+      </c>
+      <c r="D65" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" t="s">
+        <v>318</v>
+      </c>
+      <c r="F65" s="1">
+        <v>45150</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>319</v>
+      </c>
+      <c r="C66" t="s">
+        <v>320</v>
+      </c>
+      <c r="D66" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" t="s">
+        <v>318</v>
+      </c>
+      <c r="F66" s="1">
+        <v>45150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023.08.16  add: clear path from train, and doing this before removing path
</commit_message>
<xml_diff>
--- a/概要.xlsx
+++ b/概要.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codes\QtProjects\qETRC\qETRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFAD795-A8FC-4445-8539-EA39BE365630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C58EB10-AC35-4B65-BDFF-B0B0870CC42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{2D193B45-5A4E-46CA-B003-4706E03AE908}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="333">
   <si>
     <t>qETRC操作命令总表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,10 +72,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>从TrainListWidget发起的批量删除</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>添加运行图页面</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -588,10 +584,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>从导航窗口右键、或者工具栏删除单个列车对象</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>完成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1313,6 +1305,62 @@
   </si>
   <si>
     <t>RemoveTrainPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改列车径路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UpdateTrainPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AssignPathsToTrain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指定（多个）列车径路到单一车次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指定列车所属径路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移除列车所属径路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RemovePathsFromTrain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从单一列车移除（多个）列车径路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清空列车所属径路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ClearPathsFromTrain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清空指定（单一）列车的所属径路，即回到自动状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从TrainListWidget发起的批量删除；2023.08.16 增加删除前清空TrainPath的操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从导航窗口右键、或者工具栏删除单个列车对象；2023.08.16增加删除前清空列车径路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.16增加删除前清空列车</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1708,11 +1756,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5840A104-B5EE-45CC-B3E0-544B00077931}">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
+      <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1742,7 +1790,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>6</v>
@@ -1765,13 +1813,13 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3" s="1">
         <v>44379</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1779,22 +1827,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F4" s="1">
         <v>44379</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1802,22 +1850,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" s="1">
         <v>44380</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1825,10 +1873,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1840,7 +1888,7 @@
         <v>44380</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1848,22 +1896,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>57</v>
       </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7" s="1">
         <v>44381</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1871,19 +1919,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
         <v>60</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="F8" s="1">
         <v>44381</v>
       </c>
       <c r="G8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1891,19 +1939,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="F9" s="1">
         <v>44381</v>
       </c>
       <c r="G9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1911,22 +1959,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
         <v>64</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>65</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>66</v>
-      </c>
-      <c r="E10" t="s">
-        <v>67</v>
       </c>
       <c r="F10" s="1">
         <v>44382</v>
       </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1934,22 +1982,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
         <v>69</v>
       </c>
-      <c r="C11" t="s">
-        <v>70</v>
-      </c>
       <c r="D11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" t="s">
         <v>66</v>
-      </c>
-      <c r="E11" t="s">
-        <v>67</v>
       </c>
       <c r="F11" s="1">
         <v>44382</v>
       </c>
       <c r="G11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1957,22 +2005,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
         <v>104</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>105</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>106</v>
-      </c>
-      <c r="E12" t="s">
-        <v>107</v>
       </c>
       <c r="F12" s="1">
         <v>44385</v>
       </c>
       <c r="G12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1980,16 +2028,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" t="s">
         <v>106</v>
-      </c>
-      <c r="E13" t="s">
-        <v>107</v>
       </c>
       <c r="F13" s="1">
         <v>44386</v>
@@ -2000,22 +2048,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" t="s">
         <v>111</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>112</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>113</v>
-      </c>
-      <c r="E14" t="s">
-        <v>114</v>
       </c>
       <c r="F14" s="1">
         <v>44386</v>
       </c>
       <c r="G14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2023,22 +2071,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" t="s">
         <v>119</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>120</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>121</v>
-      </c>
-      <c r="E15" t="s">
-        <v>122</v>
       </c>
       <c r="F15" s="1">
         <v>44387</v>
       </c>
       <c r="G15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2046,22 +2094,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" t="s">
         <v>124</v>
       </c>
-      <c r="C16" t="s">
-        <v>125</v>
-      </c>
       <c r="D16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E16" t="s">
         <v>121</v>
-      </c>
-      <c r="E16" t="s">
-        <v>122</v>
       </c>
       <c r="F16" s="1">
         <v>44387</v>
       </c>
       <c r="G16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -2069,22 +2117,22 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" t="s">
         <v>129</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>130</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>131</v>
-      </c>
-      <c r="E17" t="s">
-        <v>132</v>
       </c>
       <c r="F17" s="1">
         <v>44388</v>
       </c>
       <c r="G17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -2092,22 +2140,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C18" t="s">
         <v>135</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>136</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>137</v>
-      </c>
-      <c r="E18" t="s">
-        <v>138</v>
       </c>
       <c r="F18" s="1">
         <v>44388</v>
       </c>
       <c r="G18" t="s">
-        <v>139</v>
+        <v>331</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -2115,22 +2163,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C19" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F19" s="4">
         <v>44484</v>
       </c>
       <c r="G19" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -2138,22 +2186,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" t="s">
+        <v>141</v>
+      </c>
+      <c r="D20" t="s">
         <v>142</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>143</v>
-      </c>
-      <c r="D20" t="s">
-        <v>144</v>
-      </c>
-      <c r="E20" t="s">
-        <v>145</v>
       </c>
       <c r="F20" s="1">
         <v>44390</v>
       </c>
       <c r="G20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -2161,22 +2209,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>150</v>
+      </c>
+      <c r="C21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D21" t="s">
         <v>152</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>153</v>
-      </c>
-      <c r="D21" t="s">
-        <v>154</v>
-      </c>
-      <c r="E21" t="s">
-        <v>155</v>
       </c>
       <c r="F21" s="1">
         <v>44391</v>
       </c>
       <c r="G21" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -2184,22 +2232,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" t="s">
         <v>158</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
         <v>159</v>
-      </c>
-      <c r="D22" t="s">
-        <v>160</v>
-      </c>
-      <c r="E22" t="s">
-        <v>161</v>
       </c>
       <c r="F22" s="1">
         <v>44392</v>
       </c>
       <c r="G22" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -2207,22 +2255,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F23" s="1">
         <v>44399</v>
       </c>
       <c r="G23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -2230,19 +2278,19 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>178</v>
+      </c>
+      <c r="C24" t="s">
+        <v>179</v>
+      </c>
+      <c r="D24" t="s">
+        <v>175</v>
+      </c>
+      <c r="E24" t="s">
+        <v>176</v>
+      </c>
+      <c r="G24" t="s">
         <v>180</v>
-      </c>
-      <c r="C24" t="s">
-        <v>181</v>
-      </c>
-      <c r="D24" t="s">
-        <v>177</v>
-      </c>
-      <c r="E24" t="s">
-        <v>178</v>
-      </c>
-      <c r="G24" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -2250,19 +2298,19 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>173</v>
+      </c>
+      <c r="C25" t="s">
+        <v>174</v>
+      </c>
+      <c r="D25" t="s">
         <v>175</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>176</v>
       </c>
-      <c r="D25" t="s">
+      <c r="G25" t="s">
         <v>177</v>
-      </c>
-      <c r="E25" t="s">
-        <v>178</v>
-      </c>
-      <c r="G25" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -2270,22 +2318,22 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C26" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D26" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E26" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F26" s="1">
         <v>44422</v>
       </c>
       <c r="G26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -2293,22 +2341,22 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
+        <v>185</v>
+      </c>
+      <c r="C27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D27" t="s">
         <v>187</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>188</v>
-      </c>
-      <c r="D27" t="s">
-        <v>189</v>
-      </c>
-      <c r="E27" t="s">
-        <v>190</v>
       </c>
       <c r="F27" s="1">
         <v>44423</v>
       </c>
       <c r="G27" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -2316,22 +2364,22 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>190</v>
+      </c>
+      <c r="C28" t="s">
+        <v>191</v>
+      </c>
+      <c r="D28" t="s">
         <v>192</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>193</v>
-      </c>
-      <c r="D28" t="s">
-        <v>194</v>
-      </c>
-      <c r="E28" t="s">
-        <v>195</v>
       </c>
       <c r="F28" s="1">
         <v>44427</v>
       </c>
       <c r="G28" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -2339,22 +2387,22 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
+        <v>195</v>
+      </c>
+      <c r="C29" t="s">
+        <v>196</v>
+      </c>
+      <c r="D29" t="s">
         <v>197</v>
       </c>
-      <c r="C29" t="s">
+      <c r="E29" t="s">
         <v>198</v>
-      </c>
-      <c r="D29" t="s">
-        <v>199</v>
-      </c>
-      <c r="E29" t="s">
-        <v>200</v>
       </c>
       <c r="F29" s="1">
         <v>44428</v>
       </c>
       <c r="G29" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -2362,22 +2410,22 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D30" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F30" s="1">
         <v>44430</v>
       </c>
       <c r="G30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -2385,22 +2433,22 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
+        <v>203</v>
+      </c>
+      <c r="C31" t="s">
+        <v>204</v>
+      </c>
+      <c r="D31" t="s">
         <v>205</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>206</v>
-      </c>
-      <c r="D31" t="s">
-        <v>207</v>
-      </c>
-      <c r="E31" t="s">
-        <v>208</v>
       </c>
       <c r="F31" s="1">
         <v>44432</v>
       </c>
       <c r="G31" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -2408,22 +2456,22 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" t="s">
+        <v>209</v>
+      </c>
+      <c r="D32" t="s">
         <v>210</v>
       </c>
-      <c r="C32" t="s">
+      <c r="E32" t="s">
         <v>211</v>
-      </c>
-      <c r="D32" t="s">
-        <v>212</v>
-      </c>
-      <c r="E32" t="s">
-        <v>213</v>
       </c>
       <c r="F32" s="1">
         <v>44433</v>
       </c>
       <c r="G32" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2431,22 +2479,22 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C33" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D33" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E33" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F33" s="1">
         <v>44434</v>
       </c>
       <c r="G33" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2454,22 +2502,22 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C34" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D34" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E34" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F34" s="1">
         <v>44435</v>
       </c>
       <c r="G34" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2477,22 +2525,22 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C35" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D35" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E35" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F35" s="1">
         <v>44435</v>
       </c>
       <c r="G35" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2500,22 +2548,22 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
+        <v>222</v>
+      </c>
+      <c r="C36" t="s">
+        <v>223</v>
+      </c>
+      <c r="D36" t="s">
         <v>224</v>
       </c>
-      <c r="C36" t="s">
+      <c r="E36" t="s">
         <v>225</v>
-      </c>
-      <c r="D36" t="s">
-        <v>226</v>
-      </c>
-      <c r="E36" t="s">
-        <v>227</v>
       </c>
       <c r="F36" s="1">
         <v>44439</v>
       </c>
       <c r="G36" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2523,22 +2571,22 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C37" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D37" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E37" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F37" s="1">
         <v>44439</v>
       </c>
       <c r="G37" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2546,22 +2594,22 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
+        <v>230</v>
+      </c>
+      <c r="C38" t="s">
+        <v>231</v>
+      </c>
+      <c r="D38" t="s">
         <v>232</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E38" t="s">
         <v>233</v>
-      </c>
-      <c r="D38" t="s">
-        <v>234</v>
-      </c>
-      <c r="E38" t="s">
-        <v>235</v>
       </c>
       <c r="F38" s="1">
         <v>44441</v>
       </c>
       <c r="G38" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2569,10 +2617,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F39" s="1">
         <v>44442</v>
@@ -2583,22 +2631,22 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
+        <v>242</v>
+      </c>
+      <c r="C40" t="s">
+        <v>243</v>
+      </c>
+      <c r="D40" t="s">
         <v>244</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" t="s">
         <v>245</v>
-      </c>
-      <c r="D40" t="s">
-        <v>246</v>
-      </c>
-      <c r="E40" t="s">
-        <v>247</v>
       </c>
       <c r="F40" s="1">
         <v>44444</v>
       </c>
       <c r="G40" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -2606,22 +2654,22 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
+        <v>247</v>
+      </c>
+      <c r="C41" t="s">
+        <v>248</v>
+      </c>
+      <c r="D41" t="s">
         <v>249</v>
       </c>
-      <c r="C41" t="s">
+      <c r="E41" t="s">
         <v>250</v>
-      </c>
-      <c r="D41" t="s">
-        <v>251</v>
-      </c>
-      <c r="E41" t="s">
-        <v>252</v>
       </c>
       <c r="F41" s="1">
         <v>44450</v>
       </c>
       <c r="G41" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -2629,22 +2677,22 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
+        <v>252</v>
+      </c>
+      <c r="C42" t="s">
+        <v>253</v>
+      </c>
+      <c r="D42" t="s">
         <v>254</v>
       </c>
-      <c r="C42" t="s">
+      <c r="E42" t="s">
         <v>255</v>
-      </c>
-      <c r="D42" t="s">
-        <v>256</v>
-      </c>
-      <c r="E42" t="s">
-        <v>257</v>
       </c>
       <c r="F42" s="1">
         <v>44453</v>
       </c>
       <c r="G42" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2652,16 +2700,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C43" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D43" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E43" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F43" s="1">
         <v>44454</v>
@@ -2672,16 +2720,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C44" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D44" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E44" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F44" s="1">
         <v>44454</v>
@@ -2692,16 +2740,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C45" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D45" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E45" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F45" s="1">
         <v>44454</v>
@@ -2712,16 +2760,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C46" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D46" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E46" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F46" s="1">
         <v>44454</v>
@@ -2732,22 +2780,22 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C47" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D47" t="s">
         <v>9</v>
       </c>
       <c r="E47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F47" s="1">
         <v>44455</v>
       </c>
       <c r="G47" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -2755,16 +2803,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C48" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D48" t="s">
         <v>9</v>
       </c>
       <c r="E48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F48" s="1">
         <v>44455</v>
@@ -2775,16 +2823,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C49" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D49" t="s">
         <v>9</v>
       </c>
       <c r="E49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F49" s="1">
         <v>44455</v>
@@ -2795,16 +2843,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C50" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D50" t="s">
         <v>9</v>
       </c>
       <c r="E50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F50" s="1">
         <v>44455</v>
@@ -2815,16 +2863,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C51" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D51" t="s">
         <v>9</v>
       </c>
       <c r="E51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F51" s="1">
         <v>44455</v>
@@ -2835,16 +2883,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C52" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D52" t="s">
         <v>9</v>
       </c>
       <c r="E52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F52" s="1">
         <v>44455</v>
@@ -2855,22 +2903,22 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C53" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D53" t="s">
         <v>9</v>
       </c>
       <c r="E53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F53" s="1">
         <v>44459</v>
       </c>
       <c r="G53" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -2878,22 +2926,22 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C54" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D54" t="s">
         <v>9</v>
       </c>
       <c r="E54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F54" s="1">
         <v>44477</v>
       </c>
       <c r="G54" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -2901,16 +2949,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C55" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D55" t="s">
         <v>9</v>
       </c>
       <c r="E55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F55" s="1">
         <v>44478</v>
@@ -2921,22 +2969,22 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C56" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D56" t="s">
         <v>9</v>
       </c>
       <c r="E56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F56" s="1">
         <v>44484</v>
       </c>
       <c r="G56" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -2944,22 +2992,22 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C57" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D57" t="s">
         <v>9</v>
       </c>
       <c r="E57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F57" s="1">
         <v>44598</v>
       </c>
       <c r="G57" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -2967,10 +3015,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C58" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D58" t="s">
         <v>9</v>
@@ -2982,7 +3030,7 @@
         <v>44703</v>
       </c>
       <c r="G58" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -2990,16 +3038,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C59" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D59" t="s">
         <v>9</v>
       </c>
       <c r="E59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F59" s="1">
         <v>44947</v>
@@ -3010,16 +3058,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C60" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D60" t="s">
         <v>9</v>
       </c>
       <c r="E60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F60" s="1">
         <v>44947</v>
@@ -3030,16 +3078,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C61" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D61" t="s">
         <v>9</v>
       </c>
       <c r="E61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F61" s="1">
         <v>44947</v>
@@ -3050,22 +3098,22 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C62" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D62" t="s">
         <v>9</v>
       </c>
       <c r="E62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F62" s="1">
         <v>44960</v>
       </c>
       <c r="G62" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
@@ -3073,10 +3121,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C63" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D63" t="s">
         <v>9</v>
@@ -3085,7 +3133,7 @@
         <v>101</v>
       </c>
       <c r="G63" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -3093,10 +3141,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C64" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D64" t="s">
         <v>9</v>
@@ -3108,47 +3156,139 @@
         <v>45079</v>
       </c>
       <c r="G64" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C65" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D65" t="s">
         <v>9</v>
       </c>
       <c r="E65" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F65" s="1">
         <v>45150</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C66" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D66" t="s">
         <v>9</v>
       </c>
       <c r="E66" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F66" s="1">
         <v>45150</v>
+      </c>
+      <c r="G66" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>319</v>
+      </c>
+      <c r="C67" t="s">
+        <v>320</v>
+      </c>
+      <c r="D67" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" t="s">
+        <v>54</v>
+      </c>
+      <c r="F67" s="1">
+        <v>45153</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>323</v>
+      </c>
+      <c r="C68" t="s">
+        <v>321</v>
+      </c>
+      <c r="D68" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" t="s">
+        <v>54</v>
+      </c>
+      <c r="F68" s="1">
+        <v>45154</v>
+      </c>
+      <c r="G68" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>324</v>
+      </c>
+      <c r="C69" t="s">
+        <v>325</v>
+      </c>
+      <c r="D69" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" t="s">
+        <v>54</v>
+      </c>
+      <c r="F69" s="1">
+        <v>45154</v>
+      </c>
+      <c r="G69" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>327</v>
+      </c>
+      <c r="C70" t="s">
+        <v>328</v>
+      </c>
+      <c r="D70" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" t="s">
+        <v>54</v>
+      </c>
+      <c r="F70" s="1">
+        <v>45154</v>
+      </c>
+      <c r="G70" t="s">
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -3177,181 +3317,181 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>49</v>
-      </c>
-      <c r="E2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
@@ -3428,69 +3568,69 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -3498,219 +3638,219 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
         <v>85</v>
       </c>
-      <c r="B14" t="s">
-        <v>86</v>
-      </c>
       <c r="C14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" t="s">
         <v>117</v>
-      </c>
-      <c r="C18" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" t="s">
         <v>98</v>
       </c>
-      <c r="B20" t="s">
-        <v>99</v>
-      </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" t="s">
         <v>95</v>
       </c>
-      <c r="B23" t="s">
-        <v>96</v>
-      </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" t="s">
         <v>92</v>
       </c>
-      <c r="B24" t="s">
-        <v>93</v>
-      </c>
       <c r="C24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C27" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B29" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C29" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C32" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023.08.22  update: re-bind upon change of path
</commit_message>
<xml_diff>
--- a/概要.xlsx
+++ b/概要.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codes\QtProjects\qETRC\qETRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C58EB10-AC35-4B65-BDFF-B0B0870CC42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141A180B-2C1D-4AB7-B04B-C2793A894E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{2D193B45-5A4E-46CA-B003-4706E03AE908}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="336">
   <si>
     <t>qETRC操作命令总表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1361,6 +1361,18 @@
   </si>
   <si>
     <t>2023.08.16增加删除前清空列车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重新铺画列车（仅限由径路铺画的）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RebindTrainsByPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通常与其他cmd伴随使用。重新铺画一组列车的运行线，仅限于使用TrainPath铺画的，不包含自动运行线的。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1756,11 +1768,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5840A104-B5EE-45CC-B3E0-544B00077931}">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
+      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3289,6 +3301,29 @@
       </c>
       <c r="G70" t="s">
         <v>329</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>333</v>
+      </c>
+      <c r="C71" t="s">
+        <v>334</v>
+      </c>
+      <c r="D71" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" t="s">
+        <v>54</v>
+      </c>
+      <c r="F71" s="1">
+        <v>45160</v>
+      </c>
+      <c r="G71" t="s">
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023.08.26  add trains to path
</commit_message>
<xml_diff>
--- a/概要.xlsx
+++ b/概要.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codes\QtProjects\qETRC\qETRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141A180B-2C1D-4AB7-B04B-C2793A894E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF63A40-6770-443A-A1F5-E9C4F30AD6D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{2D193B45-5A4E-46CA-B003-4706E03AE908}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="339">
   <si>
     <t>qETRC操作命令总表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1373,6 +1373,18 @@
   </si>
   <si>
     <t>通常与其他cmd伴随使用。重新铺画一组列车的运行线，仅限于使用TrainPath铺画的，不包含自动运行线的。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加列车到径路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddTrainsToPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加多个列车到同一个列车径路</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1768,11 +1780,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5840A104-B5EE-45CC-B3E0-544B00077931}">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A72" sqref="A72"/>
+      <selection pane="bottomLeft" activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3324,6 +3336,29 @@
       </c>
       <c r="G71" t="s">
         <v>335</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>336</v>
+      </c>
+      <c r="C72" t="s">
+        <v>337</v>
+      </c>
+      <c r="D72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" t="s">
+        <v>54</v>
+      </c>
+      <c r="F72" s="1">
+        <v>45164</v>
+      </c>
+      <c r="G72" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>